<commit_message>
Updated code for 1MG
</commit_message>
<xml_diff>
--- a/Data/AllResults.xlsx
+++ b/Data/AllResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\eclipse-workspace\QATasks\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76D1AEF-1EFA-4534-BD65-8E8702855972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02594EC5-0668-419E-AEA7-16718EB42EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,7 +344,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A361" sqref="A1:XFD361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>